<commit_message>
prep to work from home
</commit_message>
<xml_diff>
--- a/suppFiles/plasmidsAndImportantReagentsTable.xlsx
+++ b/suppFiles/plasmidsAndImportantReagentsTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared/data/Jack/DabTransporterPaper/currentSupDrafts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared/data/Jack/DabTransporterPaper/suppFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629BF6F0-BEAB-2C4F-AB33-91BD0735F3E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44F5233-4D7B-4B44-B5FB-68A1086C1CF5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50740" yWindow="3640" windowWidth="26840" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
+    <workbookView xWindow="41340" yWindow="3640" windowWidth="47380" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
   <si>
     <t>Reagent type (species) or resource</t>
   </si>
@@ -584,27 +584,6 @@
   </si>
   <si>
     <t>badabB</t>
-  </si>
-  <si>
-    <t>carrying</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>(Uniprot:</t>
-  </si>
-  <si>
-    <t>D0KWS7)</t>
-  </si>
-  <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>genes</t>
-  </si>
-  <si>
-    <t>D0KWS8)</t>
   </si>
   <si>
     <t>pFA carrying the badabA2 (locus_tag: BAS2958) and badabB2 genes (locus_tag: BAS2959)</t>
@@ -1090,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF585AB-9C60-264A-9020-DCF94C710E80}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1270,7 +1249,7 @@
         <v>77</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1287,7 +1266,7 @@
         <v>78</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1323,16 +1302,16 @@
         <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1346,7 +1325,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -1360,7 +1339,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1353,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -1388,7 +1367,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
@@ -1402,7 +1381,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
@@ -1416,65 +1395,35 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J23" t="s">
-        <v>88</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L23" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" t="s">
-        <v>90</v>
-      </c>
-      <c r="N23" t="s">
-        <v>87</v>
-      </c>
-      <c r="O23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1437,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -1502,7 +1451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -1516,7 +1465,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -1530,7 +1479,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
@@ -1544,7 +1493,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
@@ -1558,7 +1507,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
@@ -1572,7 +1521,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
@@ -1597,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:5">

</xml_diff>